<commit_message>
Update HPP Custom Impor Kertas.xlsx
</commit_message>
<xml_diff>
--- a/raw/HPP Custom Impor Kertas.xlsx
+++ b/raw/HPP Custom Impor Kertas.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Impor Kertas\HPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8FFDA8-23D9-4E80-AC6F-9A74013A6252}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695B4DB9-74FB-46C1-AECF-41EAC0755C2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9C57070C-BD48-4A1D-AFB4-7870F81B5516}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9C57070C-BD48-4A1D-AFB4-7870F81B5516}"/>
   </bookViews>
   <sheets>
     <sheet name="BM 0" sheetId="1" r:id="rId1"/>
     <sheet name="BM 5" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,23 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="48">
   <si>
     <t>Jasa Custom</t>
   </si>
   <si>
-    <t>DO Pelayaran (sesuai invoice)</t>
-  </si>
-  <si>
-    <t>Trucking (sesuai invoice)</t>
-  </si>
-  <si>
-    <t>Lolo (sesuai invoice)</t>
-  </si>
-  <si>
-    <t>Storage (sesuai invoice)</t>
-  </si>
-  <si>
     <t>Kurs</t>
   </si>
   <si>
@@ -91,19 +80,103 @@
     <t>APNK 80gsm</t>
   </si>
   <si>
-    <t>DTHC (sesuai invoice)</t>
-  </si>
-  <si>
-    <t>LSS (sesuai invoice)</t>
-  </si>
-  <si>
     <t>Canfor 80gsm</t>
   </si>
   <si>
-    <t>Bea Masuk (sesuai invoice)</t>
-  </si>
-  <si>
     <t>Harga Beli Valas</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Bulan</t>
+  </si>
+  <si>
+    <t>Invoice Penumpukan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proses Do </t>
+  </si>
+  <si>
+    <t>Invoice Behandle</t>
+  </si>
+  <si>
+    <t>Invoice Lift on Lift Off</t>
+  </si>
+  <si>
+    <t>Invoice Biaya DO</t>
+  </si>
+  <si>
+    <t>Transfer PIB</t>
+  </si>
+  <si>
+    <t>DO Pelayaran</t>
+  </si>
+  <si>
+    <t>Trucking</t>
+  </si>
+  <si>
+    <t>Jasa Custom Clearence</t>
+  </si>
+  <si>
+    <t>Jasa Behandle</t>
+  </si>
+  <si>
+    <t>Biaya extra Delivery</t>
+  </si>
+  <si>
+    <t>Print Bl Revisi Tgl BL</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Party Container</t>
+  </si>
+  <si>
+    <t>Asal Negara</t>
+  </si>
+  <si>
+    <t>Jepang</t>
+  </si>
+  <si>
+    <t>Korea Selatan</t>
+  </si>
+  <si>
+    <t>Inter Paper</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Mondi</t>
+  </si>
+  <si>
+    <t>Bosnia And Herzegovina</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Biaya Custom Clearence 2023</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>DTHC</t>
+  </si>
+  <si>
+    <t>Lift On Lift Off</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Bea Masuk</t>
   </si>
 </sst>
 </file>
@@ -116,7 +189,7 @@
     <numFmt numFmtId="164" formatCode="_-&quot;Rp&quot;* #,##0.000_-;\-&quot;Rp&quot;* #,##0.000_-;_-&quot;Rp&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +211,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,14 +237,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -337,12 +410,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -374,10 +493,44 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="42" fontId="0" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="1" builtinId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -693,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F8AE36-ED5D-42D0-968B-98F978907123}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,7 +869,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -747,11 +900,11 @@
     </row>
     <row r="3" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B3" s="22"/>
       <c r="D3" s="21" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="15"/>
@@ -762,17 +915,17 @@
     </row>
     <row r="4" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3">
-        <f>(150000)+60000+200000+100000</f>
-        <v>510000</v>
+        <f>+Sheet1!$G$27+Sheet1!$D$27+Sheet1!$M$27</f>
+        <v>591000.92307692312</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -785,11 +938,11 @@
         <v>0</v>
       </c>
       <c r="B5" s="5">
-        <f>2750000</f>
-        <v>2750000</v>
+        <f>+Sheet1!$J$27</f>
+        <v>1000000</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E5" s="16">
         <v>0.84</v>
@@ -802,14 +955,13 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5">
-        <f>2600000</f>
-        <v>2600000</v>
+        <v>2700000</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E6" s="5">
         <v>16400</v>
@@ -822,14 +974,14 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B7" s="5">
-        <f>945000</f>
-        <v>945000</v>
+        <f>+Sheet1!$F$27</f>
+        <v>846527.88461538462</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E7" s="5">
         <f>+E6*E5</f>
@@ -843,18 +995,18 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="5">
+        <f>+Sheet1!$C$27</f>
+        <v>1541221.6153846155</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="B8" s="5">
-        <f>(6672220+9197222+1198800)/3</f>
-        <v>5689414</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>8</v>
       </c>
       <c r="E8" s="5">
         <f>+B13</f>
-        <v>509.97608163265306</v>
+        <v>277.78259183673475</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
@@ -864,17 +1016,18 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B9" s="5">
-        <v>0</v>
+        <f>Sheet1!$H$27</f>
+        <v>126923.07692307692</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E9" s="5">
         <f>+E7+E8</f>
-        <v>14285.976081632652</v>
+        <v>14053.782591836734</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
@@ -884,13 +1037,13 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B10" s="10">
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E10" s="19">
         <v>0.13339999999999999</v>
@@ -903,18 +1056,18 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B11" s="10">
         <f>+SUM(B4:B10)</f>
-        <v>12494414</v>
+        <v>6805673.5000000009</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E11" s="5">
         <f>+E9*E10</f>
-        <v>1905.7492092897958</v>
+        <v>1874.7745977510203</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
@@ -924,18 +1077,18 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B12" s="12">
         <f>+E13</f>
         <v>24500</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E12" s="14">
         <f>+E9+E11</f>
-        <v>16191.725290922448</v>
+        <v>15928.557189587755</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
@@ -945,14 +1098,14 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B13" s="7">
         <f>+B11/B12</f>
-        <v>509.97608163265306</v>
+        <v>277.78259183673475</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E13" s="5">
         <v>24500</v>
@@ -965,11 +1118,11 @@
     </row>
     <row r="14" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E14" s="17">
         <f>+E13*E11</f>
-        <v>46690855.627599999</v>
+        <v>45931977.644900002</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
@@ -1022,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91248DC-3DD1-4722-9E5E-B79CCF52A66E}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,7 +1192,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -1055,29 +1208,29 @@
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="1"/>
       <c r="D3" s="21" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3">
-        <f>(150000)+60000+200000+100000</f>
-        <v>510000</v>
+        <f>+Sheet1!$G$27+Sheet1!$D$27+Sheet1!$M$27</f>
+        <v>591000.92307692312</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,12 +1238,12 @@
         <v>0</v>
       </c>
       <c r="B5" s="5">
-        <f>2750000</f>
-        <v>2750000</v>
+        <f>+Sheet1!$J$27</f>
+        <v>1000000</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E5" s="16">
         <v>1.17</v>
@@ -1098,15 +1251,14 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5">
-        <f>2600000</f>
-        <v>2600000</v>
+        <v>2700000</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E6" s="5">
         <v>16400</v>
@@ -1114,15 +1266,15 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B7" s="5">
-        <f>945000</f>
-        <v>945000</v>
+        <f>+Sheet1!$F$27</f>
+        <v>846527.88461538462</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E7" s="5">
         <f>+E6*E5</f>
@@ -1131,48 +1283,49 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="B8" s="5">
-        <f>(6672220+9197222+1198800)/3</f>
-        <v>5689414</v>
+        <f>+Sheet1!$C$27</f>
+        <v>1541221.6153846155</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E8" s="5">
         <f>+B14</f>
-        <v>1469.376081632653</v>
+        <v>1237.1825918367347</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="24">
-        <f>+E13*E7*5%</f>
-        <v>23505300</v>
+      <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="5">
+        <f>Sheet1!$H$27</f>
+        <v>126923.07692307692</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E9" s="5">
         <f>+E7+E8</f>
-        <v>20657.376081632654</v>
+        <v>20425.182591836736</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="5">
-        <v>0</v>
+      <c r="A10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="10">
+        <f>$E$7*$E$13*5/100</f>
+        <v>23505300</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E10" s="19">
         <v>0.13339999999999999</v>
@@ -1180,48 +1333,48 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B11" s="10">
         <v>0</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E11" s="5">
         <f>+E9*E10</f>
-        <v>2755.6939692897959</v>
+        <v>2724.7193577510202</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B12" s="10">
         <f>+SUM(B4:B11)</f>
-        <v>35999714</v>
+        <v>30310973.5</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E12" s="14">
         <f>+E9+E11</f>
-        <v>23413.070050922448</v>
+        <v>23149.901949587755</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B13" s="12">
-        <f>+E13</f>
+        <f>E13</f>
         <v>24500</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E13" s="5">
         <v>24500</v>
@@ -1229,27 +1382,24 @@
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B14" s="7">
-        <f>+B12/B13</f>
-        <v>1469.376081632653</v>
+        <f>B12/B13</f>
+        <v>1237.1825918367347</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E14" s="17">
         <f>+E13*E11</f>
-        <v>67514502.247600004</v>
+        <v>66755624.264899991</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1260,4 +1410,1637 @@
   <pageMargins left="0.22916666666666666" right="0.27083333333333331" top="0.125" bottom="0.40625" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9253B1FA-B7FE-4DDC-98C4-FD52ADC10D25}">
+  <dimension ref="A1:P46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <v>1</v>
+      </c>
+      <c r="B4" s="27">
+        <v>44999</v>
+      </c>
+      <c r="C4" s="28">
+        <v>812897</v>
+      </c>
+      <c r="D4" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0</v>
+      </c>
+      <c r="F4" s="28">
+        <v>888000</v>
+      </c>
+      <c r="G4" s="28">
+        <v>511000</v>
+      </c>
+      <c r="H4" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I4" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J4" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K4" s="29">
+        <v>0</v>
+      </c>
+      <c r="L4" s="29">
+        <v>0</v>
+      </c>
+      <c r="M4" s="29">
+        <v>0</v>
+      </c>
+      <c r="N4" s="28">
+        <f>+SUM(C4:M4)</f>
+        <v>6061897</v>
+      </c>
+      <c r="O4" s="29">
+        <v>1</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
+        <v>2</v>
+      </c>
+      <c r="B5" s="27">
+        <v>44988</v>
+      </c>
+      <c r="C5" s="28">
+        <v>2735797</v>
+      </c>
+      <c r="D5" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E5" s="29">
+        <v>0</v>
+      </c>
+      <c r="F5" s="28">
+        <v>100000</v>
+      </c>
+      <c r="G5" s="28">
+        <v>1750000</v>
+      </c>
+      <c r="H5" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I5" s="28">
+        <v>5200000</v>
+      </c>
+      <c r="J5" s="28">
+        <v>2000000</v>
+      </c>
+      <c r="K5" s="29">
+        <v>0</v>
+      </c>
+      <c r="L5" s="29">
+        <v>0</v>
+      </c>
+      <c r="M5" s="29">
+        <v>0</v>
+      </c>
+      <c r="N5" s="28">
+        <f>+SUM(C5:M5)</f>
+        <v>12035797</v>
+      </c>
+      <c r="O5" s="29">
+        <v>2</v>
+      </c>
+      <c r="P5" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="26">
+        <v>4</v>
+      </c>
+      <c r="B6" s="27">
+        <v>45029</v>
+      </c>
+      <c r="C6" s="28">
+        <v>3001917</v>
+      </c>
+      <c r="D6" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E6" s="29">
+        <v>0</v>
+      </c>
+      <c r="F6" s="28">
+        <f>654900+888000</f>
+        <v>1542900</v>
+      </c>
+      <c r="G6" s="28">
+        <v>661000</v>
+      </c>
+      <c r="H6" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I6" s="28">
+        <v>5200000</v>
+      </c>
+      <c r="J6" s="28">
+        <v>2000000</v>
+      </c>
+      <c r="K6" s="29">
+        <v>0</v>
+      </c>
+      <c r="L6" s="29">
+        <v>0</v>
+      </c>
+      <c r="M6" s="29">
+        <v>0</v>
+      </c>
+      <c r="N6" s="28">
+        <f>+SUM(C6:M6)</f>
+        <v>12655817</v>
+      </c>
+      <c r="O6" s="29">
+        <v>2</v>
+      </c>
+      <c r="P6" s="30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
+        <v>5</v>
+      </c>
+      <c r="B7" s="27">
+        <v>45029</v>
+      </c>
+      <c r="C7" s="28">
+        <v>2511199</v>
+      </c>
+      <c r="D7" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E7" s="29">
+        <v>0</v>
+      </c>
+      <c r="F7" s="28">
+        <v>1010500</v>
+      </c>
+      <c r="G7" s="28">
+        <v>350000</v>
+      </c>
+      <c r="H7" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I7" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J7" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K7" s="29">
+        <v>0</v>
+      </c>
+      <c r="L7" s="29">
+        <v>0</v>
+      </c>
+      <c r="M7" s="29">
+        <v>0</v>
+      </c>
+      <c r="N7" s="28">
+        <f t="shared" ref="N7:N26" si="0">+SUM(C7:M7)</f>
+        <v>7721699</v>
+      </c>
+      <c r="O7" s="29">
+        <v>1</v>
+      </c>
+      <c r="P7" s="30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
+        <v>6</v>
+      </c>
+      <c r="B8" s="27">
+        <v>45029</v>
+      </c>
+      <c r="C8" s="28">
+        <v>795971</v>
+      </c>
+      <c r="D8" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E8" s="29">
+        <v>0</v>
+      </c>
+      <c r="F8" s="28">
+        <v>699500</v>
+      </c>
+      <c r="G8" s="28">
+        <v>350000</v>
+      </c>
+      <c r="H8" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I8" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J8" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K8" s="29">
+        <v>0</v>
+      </c>
+      <c r="L8" s="29">
+        <v>0</v>
+      </c>
+      <c r="M8" s="29">
+        <v>0</v>
+      </c>
+      <c r="N8" s="28">
+        <f t="shared" si="0"/>
+        <v>5695471</v>
+      </c>
+      <c r="O8" s="29">
+        <v>1</v>
+      </c>
+      <c r="P8" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="26">
+        <v>7</v>
+      </c>
+      <c r="B9" s="27">
+        <v>45055</v>
+      </c>
+      <c r="C9" s="28">
+        <v>529848</v>
+      </c>
+      <c r="D9" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E9" s="29">
+        <v>0</v>
+      </c>
+      <c r="F9" s="28">
+        <v>888000</v>
+      </c>
+      <c r="G9" s="28">
+        <v>511000</v>
+      </c>
+      <c r="H9" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I9" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J9" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K9" s="29">
+        <v>0</v>
+      </c>
+      <c r="L9" s="29">
+        <v>0</v>
+      </c>
+      <c r="M9" s="29">
+        <v>0</v>
+      </c>
+      <c r="N9" s="28">
+        <f t="shared" si="0"/>
+        <v>5778848</v>
+      </c>
+      <c r="O9" s="29">
+        <v>1</v>
+      </c>
+      <c r="P9" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="26">
+        <v>8</v>
+      </c>
+      <c r="B10" s="27">
+        <v>45076</v>
+      </c>
+      <c r="C10" s="28">
+        <v>812898</v>
+      </c>
+      <c r="D10" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E10" s="29">
+        <v>0</v>
+      </c>
+      <c r="F10" s="28">
+        <v>999000</v>
+      </c>
+      <c r="G10" s="28">
+        <f>294440+577700</f>
+        <v>872140</v>
+      </c>
+      <c r="H10" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I10" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J10" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K10" s="29">
+        <v>0</v>
+      </c>
+      <c r="L10" s="29">
+        <v>0</v>
+      </c>
+      <c r="M10" s="28">
+        <v>100000</v>
+      </c>
+      <c r="N10" s="28">
+        <f t="shared" si="0"/>
+        <v>6634038</v>
+      </c>
+      <c r="O10" s="29">
+        <v>1</v>
+      </c>
+      <c r="P10" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="26">
+        <v>9</v>
+      </c>
+      <c r="B11" s="27">
+        <v>45093</v>
+      </c>
+      <c r="C11" s="28">
+        <v>812898</v>
+      </c>
+      <c r="D11" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E11" s="29">
+        <v>0</v>
+      </c>
+      <c r="F11" s="28">
+        <v>926850</v>
+      </c>
+      <c r="G11" s="28">
+        <v>511000</v>
+      </c>
+      <c r="H11" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I11" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J11" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K11" s="29">
+        <v>0</v>
+      </c>
+      <c r="L11" s="29">
+        <v>0</v>
+      </c>
+      <c r="M11" s="29">
+        <v>0</v>
+      </c>
+      <c r="N11" s="28">
+        <f t="shared" si="0"/>
+        <v>6100748</v>
+      </c>
+      <c r="O11" s="29">
+        <v>1</v>
+      </c>
+      <c r="P11" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="26">
+        <v>10</v>
+      </c>
+      <c r="B12" s="27">
+        <v>45093</v>
+      </c>
+      <c r="C12" s="28">
+        <v>529849</v>
+      </c>
+      <c r="D12" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E12" s="29">
+        <v>0</v>
+      </c>
+      <c r="F12" s="28">
+        <v>1010500</v>
+      </c>
+      <c r="G12" s="28">
+        <v>350000</v>
+      </c>
+      <c r="H12" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I12" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J12" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K12" s="29">
+        <v>0</v>
+      </c>
+      <c r="L12" s="29">
+        <v>0</v>
+      </c>
+      <c r="M12" s="29">
+        <v>0</v>
+      </c>
+      <c r="N12" s="28">
+        <f t="shared" si="0"/>
+        <v>5740349</v>
+      </c>
+      <c r="O12" s="29">
+        <v>1</v>
+      </c>
+      <c r="P12" s="30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
+        <v>11</v>
+      </c>
+      <c r="B13" s="27">
+        <v>45117</v>
+      </c>
+      <c r="C13" s="28">
+        <v>812899</v>
+      </c>
+      <c r="D13" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E13" s="29">
+        <v>0</v>
+      </c>
+      <c r="F13" s="28">
+        <v>960500</v>
+      </c>
+      <c r="G13" s="28">
+        <v>250000</v>
+      </c>
+      <c r="H13" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I13" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J13" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K13" s="29">
+        <v>0</v>
+      </c>
+      <c r="L13" s="29">
+        <v>0</v>
+      </c>
+      <c r="M13" s="29">
+        <v>0</v>
+      </c>
+      <c r="N13" s="28">
+        <f t="shared" si="0"/>
+        <v>5873399</v>
+      </c>
+      <c r="O13" s="29">
+        <v>1</v>
+      </c>
+      <c r="P13" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="26">
+        <v>12</v>
+      </c>
+      <c r="B14" s="27">
+        <v>45114</v>
+      </c>
+      <c r="C14" s="28">
+        <v>512921</v>
+      </c>
+      <c r="D14" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E14" s="29">
+        <v>0</v>
+      </c>
+      <c r="F14" s="28">
+        <v>754800</v>
+      </c>
+      <c r="G14" s="28">
+        <v>1287470</v>
+      </c>
+      <c r="H14" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I14" s="28">
+        <v>2500000</v>
+      </c>
+      <c r="J14" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K14" s="29">
+        <v>0</v>
+      </c>
+      <c r="L14" s="29">
+        <v>0</v>
+      </c>
+      <c r="M14" s="29">
+        <v>0</v>
+      </c>
+      <c r="N14" s="28">
+        <f t="shared" si="0"/>
+        <v>6305191</v>
+      </c>
+      <c r="O14" s="29">
+        <v>1</v>
+      </c>
+      <c r="P14" s="30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
+        <v>13</v>
+      </c>
+      <c r="B15" s="27">
+        <v>45169</v>
+      </c>
+      <c r="C15" s="28">
+        <v>812899</v>
+      </c>
+      <c r="D15" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E15" s="28">
+        <v>0</v>
+      </c>
+      <c r="F15" s="28">
+        <v>960500</v>
+      </c>
+      <c r="G15" s="28">
+        <v>475000</v>
+      </c>
+      <c r="H15" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I15" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J15" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K15" s="29">
+        <v>0</v>
+      </c>
+      <c r="L15" s="29">
+        <v>0</v>
+      </c>
+      <c r="M15" s="29">
+        <v>0</v>
+      </c>
+      <c r="N15" s="28">
+        <f t="shared" si="0"/>
+        <v>6098399</v>
+      </c>
+      <c r="O15" s="31">
+        <v>1</v>
+      </c>
+      <c r="P15" s="32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="26">
+        <v>14</v>
+      </c>
+      <c r="B16" s="27">
+        <v>45216</v>
+      </c>
+      <c r="C16" s="28">
+        <v>512921</v>
+      </c>
+      <c r="D16" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E16" s="28">
+        <v>0</v>
+      </c>
+      <c r="F16" s="28">
+        <v>757575</v>
+      </c>
+      <c r="G16" s="28">
+        <v>1304014</v>
+      </c>
+      <c r="H16" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I16" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J16" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K16" s="29">
+        <v>0</v>
+      </c>
+      <c r="L16" s="28">
+        <v>100000</v>
+      </c>
+      <c r="M16" s="29">
+        <v>0</v>
+      </c>
+      <c r="N16" s="28">
+        <f t="shared" si="0"/>
+        <v>6524510</v>
+      </c>
+      <c r="O16" s="31">
+        <v>1</v>
+      </c>
+      <c r="P16" s="32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="26">
+        <v>15</v>
+      </c>
+      <c r="B17" s="27">
+        <v>45240</v>
+      </c>
+      <c r="C17" s="28">
+        <v>812897</v>
+      </c>
+      <c r="D17" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E17" s="28">
+        <v>0</v>
+      </c>
+      <c r="F17" s="28">
+        <v>865800</v>
+      </c>
+      <c r="G17" s="28">
+        <v>100000</v>
+      </c>
+      <c r="H17" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I17" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J17" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K17" s="29">
+        <v>0</v>
+      </c>
+      <c r="L17" s="28">
+        <v>200000</v>
+      </c>
+      <c r="M17" s="29">
+        <v>0</v>
+      </c>
+      <c r="N17" s="28">
+        <f t="shared" si="0"/>
+        <v>5828697</v>
+      </c>
+      <c r="O17" s="31">
+        <v>1</v>
+      </c>
+      <c r="P17" s="32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="26">
+        <v>16</v>
+      </c>
+      <c r="B18" s="27">
+        <v>45246</v>
+      </c>
+      <c r="C18" s="28">
+        <v>3077297</v>
+      </c>
+      <c r="D18" s="28">
+        <v>200000</v>
+      </c>
+      <c r="E18" s="28">
+        <v>0</v>
+      </c>
+      <c r="F18" s="28">
+        <v>910200</v>
+      </c>
+      <c r="G18" s="28">
+        <v>100000</v>
+      </c>
+      <c r="H18" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I18" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J18" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K18" s="29">
+        <v>0</v>
+      </c>
+      <c r="L18" s="29">
+        <v>0</v>
+      </c>
+      <c r="M18" s="29">
+        <v>0</v>
+      </c>
+      <c r="N18" s="28">
+        <f t="shared" si="0"/>
+        <v>8037497</v>
+      </c>
+      <c r="O18" s="31">
+        <v>1</v>
+      </c>
+      <c r="P18" s="32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="26">
+        <v>17</v>
+      </c>
+      <c r="B19" s="27">
+        <v>45260</v>
+      </c>
+      <c r="C19" s="28">
+        <v>529849</v>
+      </c>
+      <c r="D19" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E19" s="31">
+        <v>0</v>
+      </c>
+      <c r="F19" s="28">
+        <v>1054500</v>
+      </c>
+      <c r="G19" s="28">
+        <v>650000</v>
+      </c>
+      <c r="H19" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I19" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J19" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K19" s="29">
+        <v>0</v>
+      </c>
+      <c r="L19" s="29">
+        <v>0</v>
+      </c>
+      <c r="M19" s="29">
+        <v>0</v>
+      </c>
+      <c r="N19" s="28">
+        <f t="shared" si="0"/>
+        <v>6084349</v>
+      </c>
+      <c r="O19" s="31">
+        <v>1</v>
+      </c>
+      <c r="P19" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="26">
+        <v>18</v>
+      </c>
+      <c r="B20" s="27">
+        <v>45260</v>
+      </c>
+      <c r="C20" s="28">
+        <v>812897</v>
+      </c>
+      <c r="D20" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E20" s="31">
+        <v>0</v>
+      </c>
+      <c r="F20" s="28">
+        <v>926850</v>
+      </c>
+      <c r="G20" s="28">
+        <v>511000</v>
+      </c>
+      <c r="H20" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I20" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J20" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K20" s="29">
+        <v>0</v>
+      </c>
+      <c r="L20" s="29">
+        <v>0</v>
+      </c>
+      <c r="M20" s="29">
+        <v>0</v>
+      </c>
+      <c r="N20" s="28">
+        <f t="shared" si="0"/>
+        <v>6100747</v>
+      </c>
+      <c r="O20" s="31">
+        <v>1</v>
+      </c>
+      <c r="P20" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="26">
+        <v>19</v>
+      </c>
+      <c r="B21" s="27">
+        <v>45260</v>
+      </c>
+      <c r="C21" s="28">
+        <v>1945099</v>
+      </c>
+      <c r="D21" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E21" s="31">
+        <v>0</v>
+      </c>
+      <c r="F21" s="28">
+        <v>1010500</v>
+      </c>
+      <c r="G21" s="28">
+        <v>350000</v>
+      </c>
+      <c r="H21" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I21" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J21" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K21" s="29">
+        <v>0</v>
+      </c>
+      <c r="L21" s="28">
+        <v>200000</v>
+      </c>
+      <c r="M21" s="29">
+        <v>0</v>
+      </c>
+      <c r="N21" s="28">
+        <f t="shared" si="0"/>
+        <v>7355599</v>
+      </c>
+      <c r="O21" s="31">
+        <v>1</v>
+      </c>
+      <c r="P21" s="30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="26">
+        <v>20</v>
+      </c>
+      <c r="B22" s="27">
+        <v>45276</v>
+      </c>
+      <c r="C22" s="28">
+        <v>2511198</v>
+      </c>
+      <c r="D22" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E22" s="31">
+        <v>0</v>
+      </c>
+      <c r="F22" s="28">
+        <v>926850</v>
+      </c>
+      <c r="G22" s="28">
+        <v>511000</v>
+      </c>
+      <c r="H22" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I22" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J22" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K22" s="29">
+        <v>0</v>
+      </c>
+      <c r="L22" s="29">
+        <v>0</v>
+      </c>
+      <c r="M22" s="29">
+        <v>0</v>
+      </c>
+      <c r="N22" s="28">
+        <f t="shared" si="0"/>
+        <v>7799048</v>
+      </c>
+      <c r="O22" s="31">
+        <v>1</v>
+      </c>
+      <c r="P22" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="26">
+        <v>21</v>
+      </c>
+      <c r="B23" s="27">
+        <v>45282</v>
+      </c>
+      <c r="C23" s="28">
+        <v>812898</v>
+      </c>
+      <c r="D23" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E23" s="31">
+        <v>0</v>
+      </c>
+      <c r="F23" s="28">
+        <v>888000</v>
+      </c>
+      <c r="G23" s="28">
+        <v>511000</v>
+      </c>
+      <c r="H23" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I23" s="28">
+        <v>2600000</v>
+      </c>
+      <c r="J23" s="28">
+        <v>1000000</v>
+      </c>
+      <c r="K23" s="29">
+        <v>0</v>
+      </c>
+      <c r="L23" s="29">
+        <v>0</v>
+      </c>
+      <c r="M23" s="29">
+        <v>0</v>
+      </c>
+      <c r="N23" s="28">
+        <f t="shared" si="0"/>
+        <v>6061898</v>
+      </c>
+      <c r="O23" s="31">
+        <v>1</v>
+      </c>
+      <c r="P23" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="26">
+        <v>22</v>
+      </c>
+      <c r="B24" s="27">
+        <v>45287</v>
+      </c>
+      <c r="C24" s="28">
+        <v>1556776</v>
+      </c>
+      <c r="D24" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E24" s="31">
+        <v>0</v>
+      </c>
+      <c r="F24" s="28">
+        <v>2108000</v>
+      </c>
+      <c r="G24" s="28">
+        <v>950400</v>
+      </c>
+      <c r="H24" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I24" s="28">
+        <v>5200000</v>
+      </c>
+      <c r="J24" s="28">
+        <v>2000000</v>
+      </c>
+      <c r="K24" s="29">
+        <v>0</v>
+      </c>
+      <c r="L24" s="28">
+        <v>600000</v>
+      </c>
+      <c r="M24" s="29">
+        <v>0</v>
+      </c>
+      <c r="N24" s="28">
+        <f t="shared" si="0"/>
+        <v>12665176</v>
+      </c>
+      <c r="O24" s="31">
+        <v>2</v>
+      </c>
+      <c r="P24" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="26">
+        <v>23</v>
+      </c>
+      <c r="B25" s="27">
+        <v>45287</v>
+      </c>
+      <c r="C25" s="28">
+        <f>12614585+203352</f>
+        <v>12817937</v>
+      </c>
+      <c r="D25" s="28">
+        <v>100000</v>
+      </c>
+      <c r="E25" s="29">
+        <v>0</v>
+      </c>
+      <c r="F25" s="28">
+        <v>1820400</v>
+      </c>
+      <c r="G25" s="28">
+        <v>100000</v>
+      </c>
+      <c r="H25" s="28">
+        <v>150000</v>
+      </c>
+      <c r="I25" s="28">
+        <v>5200000</v>
+      </c>
+      <c r="J25" s="28">
+        <v>2000000</v>
+      </c>
+      <c r="K25" s="29">
+        <v>0</v>
+      </c>
+      <c r="L25" s="28">
+        <v>400000</v>
+      </c>
+      <c r="M25" s="29">
+        <v>0</v>
+      </c>
+      <c r="N25" s="28">
+        <f t="shared" si="0"/>
+        <v>22588337</v>
+      </c>
+      <c r="O25" s="31">
+        <v>2</v>
+      </c>
+      <c r="P25" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="39"/>
+      <c r="C26" s="29">
+        <f>+SUM(C4:C25)</f>
+        <v>40071762</v>
+      </c>
+      <c r="D26" s="29">
+        <f t="shared" ref="D26:O26" si="1">+SUM(D4:D25)</f>
+        <v>2300000</v>
+      </c>
+      <c r="E26" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="29">
+        <f t="shared" si="1"/>
+        <v>22009725</v>
+      </c>
+      <c r="G26" s="29">
+        <f t="shared" si="1"/>
+        <v>12966024</v>
+      </c>
+      <c r="H26" s="29">
+        <f t="shared" si="1"/>
+        <v>3300000</v>
+      </c>
+      <c r="I26" s="29">
+        <f t="shared" si="1"/>
+        <v>67500000</v>
+      </c>
+      <c r="J26" s="29">
+        <f t="shared" si="1"/>
+        <v>26000000</v>
+      </c>
+      <c r="K26" s="29">
+        <f t="shared" ref="K26" si="2">+SUM(K4:K25)</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="29">
+        <f t="shared" ref="L26" si="3">+SUM(L4:L25)</f>
+        <v>1500000</v>
+      </c>
+      <c r="M26" s="29">
+        <f t="shared" ref="M26" si="4">+SUM(M4:M25)</f>
+        <v>100000</v>
+      </c>
+      <c r="N26" s="28">
+        <f t="shared" si="0"/>
+        <v>175747511</v>
+      </c>
+      <c r="O26" s="29">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="P26" s="30"/>
+    </row>
+    <row r="27" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="40"/>
+      <c r="C27" s="33">
+        <f>IF(C26&gt;0,C26/$O$26,0)</f>
+        <v>1541221.6153846155</v>
+      </c>
+      <c r="D27" s="33">
+        <f>IF(D26&gt;0,D26/$O$26,0)</f>
+        <v>88461.538461538468</v>
+      </c>
+      <c r="E27" s="33">
+        <f>IF(E26&gt;0,E26/$O$26,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="33">
+        <f>IF(F26&gt;0,F26/$O$26,0)</f>
+        <v>846527.88461538462</v>
+      </c>
+      <c r="G27" s="33">
+        <f>IF(G26&gt;0,G26/$O$26,0)</f>
+        <v>498693.23076923075</v>
+      </c>
+      <c r="H27" s="33">
+        <f>IF(H26&gt;0,H26/$O$26,0)</f>
+        <v>126923.07692307692</v>
+      </c>
+      <c r="I27" s="33">
+        <f>IF(I26&gt;0,I26/$O$26,0)</f>
+        <v>2596153.846153846</v>
+      </c>
+      <c r="J27" s="33">
+        <f>IF(J26&gt;0,J26/$O$26,0)</f>
+        <v>1000000</v>
+      </c>
+      <c r="K27" s="33">
+        <f t="shared" ref="K27:M27" si="5">IF(K26&gt;0,K26/$O$26,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L27" s="33">
+        <f t="shared" si="5"/>
+        <v>57692.307692307695</v>
+      </c>
+      <c r="M27" s="33">
+        <f t="shared" si="5"/>
+        <v>3846.1538461538462</v>
+      </c>
+      <c r="N27" s="33">
+        <f>IF(N26&gt;0,N26/$O$26,0)</f>
+        <v>6759519.653846154</v>
+      </c>
+      <c r="O27" s="33"/>
+      <c r="P27" s="41"/>
+    </row>
+    <row r="28" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="35"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="35"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
+      <c r="N30" s="35"/>
+      <c r="O30" s="35"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="35"/>
+      <c r="O31" s="35"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="35"/>
+      <c r="N32" s="35"/>
+      <c r="O32" s="35"/>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
+      <c r="L34" s="35"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="35"/>
+      <c r="O34" s="35"/>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="35"/>
+    </row>
+    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="35"/>
+      <c r="N36" s="35"/>
+      <c r="O36" s="35"/>
+    </row>
+    <row r="37" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="35"/>
+    </row>
+    <row r="38" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="35"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="35"/>
+      <c r="L38" s="35"/>
+      <c r="M38" s="35"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="35"/>
+    </row>
+    <row r="39" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="35"/>
+      <c r="L39" s="35"/>
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
+    </row>
+    <row r="40" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="35"/>
+      <c r="M40" s="35"/>
+      <c r="N40" s="35"/>
+      <c r="O40" s="35"/>
+    </row>
+    <row r="41" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="35"/>
+      <c r="L41" s="35"/>
+      <c r="M41" s="35"/>
+      <c r="N41" s="35"/>
+      <c r="O41" s="35"/>
+    </row>
+    <row r="42" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="35"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="35"/>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="35"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="35"/>
+    </row>
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="35"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="35"/>
+      <c r="O44" s="35"/>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="35"/>
+      <c r="L45" s="35"/>
+      <c r="M45" s="35"/>
+      <c r="N45" s="35"/>
+      <c r="O45" s="35"/>
+    </row>
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="35"/>
+      <c r="L46" s="35"/>
+      <c r="M46" s="35"/>
+      <c r="N46" s="35"/>
+      <c r="O46" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>